<commit_message>
added Present Perfect Continuous into BigBen
</commit_message>
<xml_diff>
--- a/English/BigBen/stative verbs.xlsx
+++ b/English/BigBen/stative verbs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Senses</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>recognise   (узнавать)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stay (останавливаться)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> exist (существовать)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> remain (оставаться)</t>
   </si>
 </sst>
 </file>
@@ -341,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -373,6 +382,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,8 +394,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,7 +716,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,20 +730,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -891,30 +918,36 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="13" t="s">
+    <row r="19" spans="1:5" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="13" t="s">
+    <row r="20" spans="1:5" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="15"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="14" t="s">
+    <row r="21" spans="1:5" s="25" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="26"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="22" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added defining into BigBen and amended stative verbs
</commit_message>
<xml_diff>
--- a/English/BigBen/stative verbs.xlsx
+++ b/English/BigBen/stative verbs.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$E$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$O$18</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Senses</t>
   </si>
@@ -148,13 +148,18 @@
   </si>
   <si>
     <t xml:space="preserve"> remain (оставаться)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S T A T I V E  OR  D I N A M I C
+depends on context
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,13 +167,6 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0D0D0D"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="16"/>
@@ -243,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -346,71 +344,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,247 +771,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
     <col min="5" max="5" width="51.42578125" customWidth="1"/>
     <col min="6" max="6" width="31.42578125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" customWidth="1"/>
+    <col min="8" max="8" width="71.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="H1" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
       <c r="C5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5"/>
       <c r="C8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="11" t="s">
+    <row r="9" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="16"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="13" t="s">
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="23" t="s">
+    <row r="16" spans="1:11" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="21" t="s">
+      <c r="D16" s="18"/>
+      <c r="E16" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="23" t="s">
+    <row r="17" spans="1:5" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="21" t="s">
+      <c r="D17" s="18"/>
+      <c r="E17" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="25" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="26" t="s">
+    <row r="18" spans="1:5" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="22" t="s">
+      <c r="D18" s="18"/>
+      <c r="E18" s="16" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H1:H3"/>
   </mergeCells>
   <pageMargins left="1.1023622047244095" right="1.1023622047244095" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="76" orientation="landscape" r:id="rId1"/>

</xml_diff>